<commit_message>
server: add Categories controller
</commit_message>
<xml_diff>
--- a/server/APIs documentation.xlsx
+++ b/server/APIs documentation.xlsx
@@ -137,8 +137,7 @@
   },
   ... 
   ]
-}
-</t>
+}</t>
   </si>
   <si>
     <t>Thông tin giống như 1 mảng course nhưng
@@ -611,10 +610,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G65536"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -629,10 +628,8 @@
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="14.4285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -640,73 +637,66 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F4" s="2" t="s">
+    <row r="2" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+    <row r="7" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
@@ -714,170 +704,188 @@
         <v>15</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="F9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5"/>
+      <c r="B11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="14" t="s">
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5"/>
+      <c r="B12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D12" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E12" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="17"/>
-    </row>
-    <row r="13" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="9" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5"/>
+      <c r="B14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="14" t="s">
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5"/>
+      <c r="B15" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C15" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D15" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15" t="s">
+      <c r="E15" s="14"/>
+      <c r="F15" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19" t="s">
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B16" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-      <c r="B16" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="19"/>
+      <c r="B17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>